<commit_message>
big commit of result files
</commit_message>
<xml_diff>
--- a/scalpel/typeinfer/evaluation/evaluation_outputs/521xueweihan__HelloGitHub.xlsx
+++ b/scalpel/typeinfer/evaluation/evaluation_outputs/521xueweihan__HelloGitHub.xlsx
@@ -29,12 +29,32 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFA500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00008000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +75,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,551 +483,883 @@
           <t>Scalpel Type</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>get_data</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>{'any', 'List[any]'}</t>
         </is>
       </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>get_data</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Any</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>any</t>
+        </is>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>get_all_data</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>list</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>{'List[any]'}</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>get_all_data</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>list</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>List[any]</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>check_condition</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>Optional</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>{'bool'}</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="F6" s="4" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>check_condition</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>analyze</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>list</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>{'List[any]'}</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>analyze</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>list</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>List[any]</t>
+        </is>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>get_stars</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>List</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>{'any', 'List[any]'}</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>get_stars</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>any</t>
+        </is>
+      </c>
+      <c r="F11" s="4" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>make_content</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D12" s="2" t="inlineStr">
         <is>
           <t>List</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>{'List[any]'}</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>make_content</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>List</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>List[any]</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
         <is>
           <t>get_data</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D14" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E14" s="2" t="inlineStr">
         <is>
           <t>any</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>check_condition</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D15" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E15" s="2" t="inlineStr">
         <is>
           <t>any</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>analyze</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D16" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E16" s="2" t="inlineStr">
         <is>
           <t>any</t>
         </is>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>get_stars</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D17" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E17" s="2" t="inlineStr">
         <is>
           <t>any</t>
         </is>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
         <is>
           <t>send_email</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D18" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E18" s="2" t="inlineStr">
         <is>
           <t>any</t>
         </is>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>github_bot.py</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>github_bot.py</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
         <is>
           <t>send_email</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D19" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E19" s="2" t="inlineStr">
         <is>
           <t>any</t>
         </is>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>make_content.py</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C20" s="2" t="inlineStr">
         <is>
           <t>check_path</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D20" s="2" t="inlineStr">
         <is>
           <t>bool</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E20" s="2" t="inlineStr">
         <is>
           <t>{'bool'}</t>
         </is>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>make_content.py</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C21" s="2" t="inlineStr">
         <is>
           <t>check_path</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>bool</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>make_content.py</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>check_path</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E22" s="2" t="inlineStr">
         <is>
           <t>any</t>
         </is>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>make_content.py</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C23" s="2" t="inlineStr">
         <is>
           <t>read_file</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D23" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E23" s="2" t="inlineStr">
         <is>
           <t>any</t>
         </is>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
         <is>
           <t>make_content.py</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C24" s="2" t="inlineStr">
         <is>
           <t>write_file</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D24" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E24" s="2" t="inlineStr">
         <is>
           <t>any</t>
         </is>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>make_content.py</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C25" s="2" t="inlineStr">
         <is>
           <t>write_file</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D25" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E25" s="2" t="inlineStr">
         <is>
           <t>any</t>
         </is>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
         <is>
           <t>make_content.py</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C26" s="2" t="inlineStr">
         <is>
           <t>make_content</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="D26" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E26" s="2" t="inlineStr">
         <is>
           <t>int</t>
         </is>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>521xueweihan__HelloGitHub</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
+      <c r="F26" s="5" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>521xueweihan__HelloGitHub</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
         <is>
           <t>make_content.py</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C27" s="2" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D27" s="2" t="inlineStr">
         <is>
           <t>Any</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E27" s="2" t="inlineStr">
         <is>
           <t>any</t>
         </is>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>PyType Total:</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>21</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Scalpel Total:</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>15</v>
-      </c>
-      <c r="E21" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Accuracy</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>71.43000000000001</v>
-      </c>
-      <c r="E22" t="inlineStr"/>
+      <c r="F27" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>Total comparisons:</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>PyType Wins:</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>Scalpel Wins:</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr"/>
+      <c r="B29" s="2" t="inlineStr"/>
+      <c r="C29" s="2" t="inlineStr"/>
+      <c r="D29" s="2" t="inlineStr"/>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>Accuracy over PyType</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>33.33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
adding all pytype stubs and extra row to resultant output
</commit_message>
<xml_diff>
--- a/scalpel/typeinfer/evaluation/evaluation_outputs/521xueweihan__HelloGitHub.xlsx
+++ b/scalpel/typeinfer/evaluation/evaluation_outputs/521xueweihan__HelloGitHub.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1350,14 +1350,28 @@
     <row r="29">
       <c r="A29" s="2" t="inlineStr"/>
       <c r="B29" s="2" t="inlineStr"/>
-      <c r="C29" s="2" t="inlineStr"/>
-      <c r="D29" s="2" t="inlineStr"/>
-      <c r="E29" s="2" t="inlineStr">
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>Scalpel Accuracy:</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>766.67</v>
+      </c>
+      <c r="E29" s="2" t="inlineStr"/>
+      <c r="F29" s="2" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr"/>
+      <c r="B30" s="2" t="inlineStr"/>
+      <c r="C30" s="2" t="inlineStr"/>
+      <c r="D30" s="2" t="inlineStr"/>
+      <c r="E30" s="2" t="inlineStr">
         <is>
           <t>Accuracy over PyType</t>
         </is>
       </c>
-      <c r="F29" s="2" t="n">
+      <c r="F30" s="2" t="n">
         <v>33.33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed error causing the output accuracy to be incorrect
</commit_message>
<xml_diff>
--- a/scalpel/typeinfer/evaluation/evaluation_outputs/521xueweihan__HelloGitHub.xlsx
+++ b/scalpel/typeinfer/evaluation/evaluation_outputs/521xueweihan__HelloGitHub.xlsx
@@ -512,7 +512,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>{'any', 'List[any]'}</t>
+          <t>{'List[any]', 'any'}</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
@@ -544,7 +544,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>any</t>
+          <t>List[any]</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
@@ -768,7 +768,7 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>{'any', 'List[any]'}</t>
+          <t>{'List[any]', 'any'}</t>
         </is>
       </c>
       <c r="F10" s="3" t="inlineStr">
@@ -800,12 +800,12 @@
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>any</t>
-        </is>
-      </c>
-      <c r="F11" s="4" t="inlineStr">
-        <is>
-          <t>Loss</t>
+          <t>List[any]</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -1336,7 +1336,7 @@
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
@@ -1350,16 +1350,16 @@
     <row r="29">
       <c r="A29" s="2" t="inlineStr"/>
       <c r="B29" s="2" t="inlineStr"/>
-      <c r="C29" s="2" t="inlineStr">
+      <c r="C29" s="2" t="inlineStr"/>
+      <c r="D29" s="2" t="inlineStr"/>
+      <c r="E29" s="2" t="inlineStr">
         <is>
           <t>Scalpel Accuracy:</t>
         </is>
       </c>
-      <c r="D29" s="2" t="n">
-        <v>766.67</v>
-      </c>
-      <c r="E29" s="2" t="inlineStr"/>
-      <c r="F29" s="2" t="inlineStr"/>
+      <c r="F29" s="2" t="n">
+        <v>92.31</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr"/>
@@ -1368,11 +1368,11 @@
       <c r="D30" s="2" t="inlineStr"/>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>Accuracy over PyType</t>
+          <t>Accuracy vs PyType</t>
         </is>
       </c>
       <c r="F30" s="2" t="n">
-        <v>33.33</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>